<commit_message>
added the all updated files
</commit_message>
<xml_diff>
--- a/Javascript-questionnaire.xlsx
+++ b/Javascript-questionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="187">
   <si>
     <t>Ans</t>
   </si>
@@ -1429,6 +1429,12 @@
   </si>
   <si>
     <t xml:space="preserve">useState, useContext, and useEffect are all hooks provided by the React library, </t>
+  </si>
+  <si>
+    <t>One is state, another one is callback</t>
+  </si>
+  <si>
+    <t>Infinite Loop</t>
   </si>
 </sst>
 </file>
@@ -1532,14 +1538,6 @@
       <family val="3"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF040C28"/>
       <name val="Calibri"/>
@@ -1592,6 +1590,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1701,31 +1705,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2024,7 +2026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B210"/>
   <sheetViews>
-    <sheetView topLeftCell="A198" workbookViewId="0">
+    <sheetView topLeftCell="A193" workbookViewId="0">
       <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>
@@ -3019,7 +3021,7 @@
       <c r="A203" s="8">
         <v>40</v>
       </c>
-      <c r="B203" s="33" t="s">
+      <c r="B203" s="32" t="s">
         <v>142</v>
       </c>
     </row>
@@ -3035,7 +3037,7 @@
       <c r="A206" s="8">
         <v>41</v>
       </c>
-      <c r="B206" s="33" t="s">
+      <c r="B206" s="32" t="s">
         <v>172</v>
       </c>
     </row>
@@ -3048,7 +3050,7 @@
       <c r="A209" s="8">
         <v>42</v>
       </c>
-      <c r="B209" s="33" t="s">
+      <c r="B209" s="32" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3071,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3151,7 +3153,7 @@
       <c r="A12" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3348,9 +3350,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" ht="16.5">
       <c r="A51" s="30" t="s">
         <v>169</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3365,7 +3370,9 @@
       <c r="A54" s="30" t="s">
         <v>148</v>
       </c>
-      <c r="B54" s="32"/>
+      <c r="B54" s="24" t="s">
+        <v>185</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>